<commit_message>
New commit from notepad
</commit_message>
<xml_diff>
--- a/VS680_Scripts/vs680scripts/launchTimeTest/BestTestAppLaunchTime/Touch启动时间测试用例.xlsx
+++ b/VS680_Scripts/vs680scripts/launchTimeTest/BestTestAppLaunchTime/Touch启动时间测试用例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\VS680_Scripts\vs680scripts\launchTimeTest\BestTestAppLaunchTime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\pythonProject_seevision\VS680_Scripts\vs680scripts\launchTimeTest\BestTestAppLaunchTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8002A1-64FD-4872-BCE9-1F72720B5669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017C4AD8-3953-4022-8B89-D2EE4B94EABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1190" windowWidth="12800" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Touch启动时间测试" sheetId="1" r:id="rId1"/>
@@ -653,18 +653,18 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
-    <col min="2" max="2" width="21.36328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="8.77734375" style="4"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="4"/>
     <col min="6" max="6" width="53" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="4"/>
+    <col min="7" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -707,7 +707,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -727,7 +727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -747,7 +747,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -767,7 +767,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -787,7 +787,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -807,7 +807,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -827,7 +827,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -847,7 +847,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -867,7 +867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -887,7 +887,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -907,7 +907,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -927,7 +927,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -947,7 +947,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -967,7 +967,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -987,7 +987,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>

</xml_diff>